<commit_message>
update 07 10 2021
</commit_message>
<xml_diff>
--- a/rekap data uang kas kecil - asrama.xlsx
+++ b/rekap data uang kas kecil - asrama.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yofandi Riki Winata\Documents\yofandi\rekap data - uang galon, parkir, bumbu asrama\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yofandi Riki Winata\Documents\yofandi\rekap data - uang galon, parkir, bumbu asrama\uangasrama\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D91FADE5-BFF8-450C-84CC-56F83A96CE5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBDE82F6-B4E1-407D-9547-BCDDBBB97330}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{C456B771-9DF8-4725-AC5F-E2624C050843}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
   <si>
     <t>Kas Kecil - Asrama STTHF</t>
   </si>
@@ -71,6 +71,27 @@
   </si>
   <si>
     <t>petrus</t>
+  </si>
+  <si>
+    <t>uang beli garam</t>
+  </si>
+  <si>
+    <t xml:space="preserve">peter </t>
+  </si>
+  <si>
+    <t>uang beli minyak 2L</t>
+  </si>
+  <si>
+    <t>uang beli nasi padang 11</t>
+  </si>
+  <si>
+    <t>valen</t>
+  </si>
+  <si>
+    <t>uang beli susu</t>
+  </si>
+  <si>
+    <t>tondo</t>
   </si>
 </sst>
 </file>
@@ -79,8 +100,8 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
-    <numFmt numFmtId="168" formatCode="[$-421]dd\ mmmm\ yyyy;@"/>
-    <numFmt numFmtId="169" formatCode="_([$Rp-421]* #,##0.00_);_([$Rp-421]* \(#,##0.00\);_([$Rp-421]* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="_([$Rp-421]* #,##0.00_);_([$Rp-421]* \(#,##0.00\);_([$Rp-421]* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="166" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -149,12 +170,6 @@
   </cellStyleXfs>
   <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -168,8 +183,14 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -485,15 +506,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1137C53-0063-4FE4-9637-7E05AFF16C56}">
-  <dimension ref="A1:N10"/>
+  <dimension ref="A1:N74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="34.7109375" style="7" customWidth="1"/>
+    <col min="1" max="1" width="34.7109375" style="5" customWidth="1"/>
     <col min="2" max="2" width="31.42578125" customWidth="1"/>
     <col min="3" max="3" width="33.85546875" customWidth="1"/>
     <col min="4" max="4" width="27.85546875" customWidth="1"/>
@@ -502,141 +523,141 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
-      <c r="J1" s="4"/>
-      <c r="K1" s="4"/>
-      <c r="L1" s="4"/>
-      <c r="M1" s="4"/>
-      <c r="N1" s="4"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
+      <c r="L1" s="2"/>
+      <c r="M1" s="2"/>
+      <c r="N1" s="2"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
-      <c r="I2" s="4"/>
-      <c r="J2" s="4"/>
-      <c r="K2" s="4"/>
-      <c r="L2" s="4"/>
-      <c r="M2" s="4"/>
-      <c r="N2" s="4"/>
+      <c r="A2" s="8"/>
+      <c r="B2" s="8"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="8"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2"/>
+      <c r="L2" s="2"/>
+      <c r="M2" s="2"/>
+      <c r="N2" s="2"/>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="4"/>
-      <c r="H3" s="4"/>
-      <c r="I3" s="4"/>
-      <c r="J3" s="4"/>
-      <c r="K3" s="4"/>
-      <c r="L3" s="4"/>
-      <c r="M3" s="4"/>
-      <c r="N3" s="4"/>
+      <c r="A3" s="8"/>
+      <c r="B3" s="8"/>
+      <c r="C3" s="8"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="8"/>
+      <c r="F3" s="8"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
+      <c r="L3" s="2"/>
+      <c r="M3" s="2"/>
+      <c r="N3" s="2"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A4" s="1"/>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="4"/>
-      <c r="H4" s="4"/>
-      <c r="I4" s="4"/>
-      <c r="J4" s="4"/>
-      <c r="K4" s="4"/>
-      <c r="L4" s="4"/>
-      <c r="M4" s="4"/>
-      <c r="N4" s="4"/>
+      <c r="A4" s="8"/>
+      <c r="B4" s="8"/>
+      <c r="C4" s="8"/>
+      <c r="D4" s="8"/>
+      <c r="E4" s="8"/>
+      <c r="F4" s="8"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
+      <c r="K4" s="2"/>
+      <c r="L4" s="2"/>
+      <c r="M4" s="2"/>
+      <c r="N4" s="2"/>
     </row>
     <row r="5" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="5"/>
-      <c r="H5" s="5"/>
-      <c r="I5" s="5"/>
-      <c r="J5" s="5"/>
-      <c r="K5" s="5"/>
-      <c r="L5" s="5"/>
-      <c r="M5" s="5"/>
-      <c r="N5" s="5"/>
+      <c r="B5" s="9"/>
+      <c r="C5" s="9"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="9"/>
+      <c r="F5" s="9"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
+      <c r="K5" s="3"/>
+      <c r="L5" s="3"/>
+      <c r="M5" s="3"/>
+      <c r="N5" s="3"/>
     </row>
     <row r="6" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="2"/>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="5"/>
-      <c r="H6" s="5"/>
-      <c r="I6" s="5"/>
-      <c r="J6" s="5"/>
-      <c r="K6" s="5"/>
-      <c r="L6" s="5"/>
-      <c r="M6" s="5"/>
-      <c r="N6" s="5"/>
+      <c r="A6" s="9"/>
+      <c r="B6" s="9"/>
+      <c r="C6" s="9"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="9"/>
+      <c r="F6" s="9"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
+      <c r="K6" s="3"/>
+      <c r="L6" s="3"/>
+      <c r="M6" s="3"/>
+      <c r="N6" s="3"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A7" s="7" t="s">
+      <c r="A7" s="5" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:14" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A8" s="6" t="s">
+      <c r="A8" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="D8" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E8" s="3" t="s">
+      <c r="E8" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="F8" s="3" t="s">
+      <c r="F8" s="1" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A9" s="8">
+      <c r="A9" s="7">
         <v>44473</v>
       </c>
-      <c r="B9" s="9">
+      <c r="B9" s="6">
         <v>500000</v>
       </c>
-      <c r="C9" s="9">
+      <c r="C9" s="6">
         <v>0</v>
       </c>
-      <c r="D9" s="9">
+      <c r="D9" s="6">
         <f>B9-C9</f>
         <v>500000</v>
       </c>
@@ -648,16 +669,16 @@
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A10" s="8">
+      <c r="A10" s="7">
         <v>44474</v>
       </c>
-      <c r="B10" s="9">
+      <c r="B10" s="6">
         <v>0</v>
       </c>
-      <c r="C10" s="9">
+      <c r="C10" s="6">
         <v>70500</v>
       </c>
-      <c r="D10" s="9">
+      <c r="D10" s="6">
         <f>D9+B10-C10</f>
         <v>429500</v>
       </c>
@@ -667,6 +688,326 @@
       <c r="F10" t="s">
         <v>12</v>
       </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A11" s="7">
+        <v>44475</v>
+      </c>
+      <c r="B11" s="6">
+        <v>0</v>
+      </c>
+      <c r="C11" s="6">
+        <v>17500</v>
+      </c>
+      <c r="D11" s="6">
+        <f t="shared" ref="D11:D14" si="0">D10+B11-C11</f>
+        <v>412000</v>
+      </c>
+      <c r="E11" t="s">
+        <v>13</v>
+      </c>
+      <c r="F11" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A12" s="7">
+        <v>44475</v>
+      </c>
+      <c r="B12" s="6">
+        <v>0</v>
+      </c>
+      <c r="C12" s="6">
+        <v>35700</v>
+      </c>
+      <c r="D12" s="6">
+        <f t="shared" si="0"/>
+        <v>376300</v>
+      </c>
+      <c r="E12" t="s">
+        <v>15</v>
+      </c>
+      <c r="F12" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A13" s="7">
+        <v>44476</v>
+      </c>
+      <c r="B13" s="6">
+        <v>0</v>
+      </c>
+      <c r="C13" s="6">
+        <v>154000</v>
+      </c>
+      <c r="D13" s="6">
+        <f t="shared" si="0"/>
+        <v>222300</v>
+      </c>
+      <c r="E13" t="s">
+        <v>16</v>
+      </c>
+      <c r="F13" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A14" s="7">
+        <v>44476</v>
+      </c>
+      <c r="B14" s="6">
+        <v>0</v>
+      </c>
+      <c r="C14" s="6">
+        <v>100000</v>
+      </c>
+      <c r="D14" s="6">
+        <f t="shared" si="0"/>
+        <v>122300</v>
+      </c>
+      <c r="E14" t="s">
+        <v>18</v>
+      </c>
+      <c r="F14" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A15" s="7"/>
+      <c r="B15" s="6"/>
+      <c r="C15" s="6"/>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A16" s="7"/>
+      <c r="B16" s="6"/>
+      <c r="C16" s="6"/>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="7"/>
+      <c r="B17" s="6"/>
+      <c r="C17" s="6"/>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="7"/>
+      <c r="B18" s="6"/>
+      <c r="C18" s="6"/>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="7"/>
+      <c r="B19" s="6"/>
+      <c r="C19" s="6"/>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="7"/>
+      <c r="B20" s="6"/>
+      <c r="C20" s="6"/>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="7"/>
+      <c r="B21" s="6"/>
+      <c r="C21" s="6"/>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="7"/>
+      <c r="B22" s="6"/>
+      <c r="C22" s="6"/>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="7"/>
+      <c r="B23" s="6"/>
+      <c r="C23" s="6"/>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="7"/>
+      <c r="B24" s="6"/>
+      <c r="C24" s="6"/>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="7"/>
+      <c r="B25" s="6"/>
+      <c r="C25" s="6"/>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="7"/>
+      <c r="B26" s="6"/>
+      <c r="C26" s="6"/>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="7"/>
+      <c r="B27" s="6"/>
+      <c r="C27" s="6"/>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="7"/>
+      <c r="B28" s="6"/>
+      <c r="C28" s="6"/>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="7"/>
+      <c r="B29" s="6"/>
+      <c r="C29" s="6"/>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="7"/>
+      <c r="B30" s="6"/>
+      <c r="C30" s="6"/>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="7"/>
+      <c r="B31" s="6"/>
+      <c r="C31" s="6"/>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="7"/>
+      <c r="B32" s="6"/>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" s="7"/>
+      <c r="B33" s="6"/>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" s="7"/>
+      <c r="B34" s="6"/>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" s="7"/>
+      <c r="B35" s="6"/>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" s="7"/>
+      <c r="B36" s="6"/>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" s="7"/>
+      <c r="B37" s="6"/>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" s="7"/>
+      <c r="B38" s="6"/>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" s="7"/>
+      <c r="B39" s="6"/>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" s="7"/>
+      <c r="B40" s="6"/>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" s="7"/>
+      <c r="B41" s="6"/>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" s="7"/>
+      <c r="B42" s="6"/>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" s="7"/>
+      <c r="B43" s="6"/>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" s="7"/>
+      <c r="B44" s="6"/>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" s="7"/>
+      <c r="B45" s="6"/>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" s="7"/>
+      <c r="B46" s="6"/>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" s="7"/>
+      <c r="B47" s="6"/>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" s="7"/>
+      <c r="B48" s="6"/>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" s="7"/>
+      <c r="B49" s="6"/>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" s="7"/>
+      <c r="B50" s="6"/>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" s="7"/>
+      <c r="B51" s="6"/>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" s="7"/>
+      <c r="B52" s="6"/>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" s="7"/>
+      <c r="B53" s="6"/>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54" s="7"/>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55" s="7"/>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56" s="7"/>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57" s="7"/>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A58" s="7"/>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59" s="7"/>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A60" s="7"/>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A61" s="7"/>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A62" s="7"/>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A63" s="7"/>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A64" s="7"/>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A65" s="7"/>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A66" s="7"/>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A67" s="7"/>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A68" s="7"/>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A69" s="7"/>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A70" s="7"/>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A71" s="7"/>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A72" s="7"/>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A73" s="7"/>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A74" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
update 09 10 2021
</commit_message>
<xml_diff>
--- a/rekap data uang kas kecil - asrama.xlsx
+++ b/rekap data uang kas kecil - asrama.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yofandi Riki Winata\Documents\yofandi\rekap data - uang galon, parkir, bumbu asrama\uangasrama\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBDE82F6-B4E1-407D-9547-BCDDBBB97330}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25E2A502-7305-4B37-B81A-A1A4373D4A81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{C456B771-9DF8-4725-AC5F-E2624C050843}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="24">
   <si>
     <t>Kas Kecil - Asrama STTHF</t>
   </si>
@@ -92,6 +92,18 @@
   </si>
   <si>
     <t>tondo</t>
+  </si>
+  <si>
+    <t>uang karcis juanda</t>
+  </si>
+  <si>
+    <t>Tondo</t>
+  </si>
+  <si>
+    <t>uang beli bensin pertalite</t>
+  </si>
+  <si>
+    <t>yofandi</t>
   </si>
 </sst>
 </file>
@@ -509,7 +521,7 @@
   <dimension ref="A1:N74"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -700,7 +712,7 @@
         <v>17500</v>
       </c>
       <c r="D11" s="6">
-        <f t="shared" ref="D11:D14" si="0">D10+B11-C11</f>
+        <f t="shared" ref="D11:D16" si="0">D10+B11-C11</f>
         <v>412000</v>
       </c>
       <c r="E11" t="s">
@@ -760,11 +772,11 @@
         <v>0</v>
       </c>
       <c r="C14" s="6">
-        <v>100000</v>
+        <v>101200</v>
       </c>
       <c r="D14" s="6">
         <f t="shared" si="0"/>
-        <v>122300</v>
+        <v>121100</v>
       </c>
       <c r="E14" t="s">
         <v>18</v>
@@ -774,14 +786,46 @@
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A15" s="7"/>
-      <c r="B15" s="6"/>
-      <c r="C15" s="6"/>
+      <c r="A15" s="7">
+        <v>44476</v>
+      </c>
+      <c r="B15" s="6">
+        <v>0</v>
+      </c>
+      <c r="C15" s="6">
+        <v>13000</v>
+      </c>
+      <c r="D15" s="6">
+        <f t="shared" si="0"/>
+        <v>108100</v>
+      </c>
+      <c r="E15" t="s">
+        <v>20</v>
+      </c>
+      <c r="F15" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A16" s="7"/>
-      <c r="B16" s="6"/>
-      <c r="C16" s="6"/>
+      <c r="A16" s="7">
+        <v>44477</v>
+      </c>
+      <c r="B16" s="6">
+        <v>0</v>
+      </c>
+      <c r="C16" s="6">
+        <v>10000</v>
+      </c>
+      <c r="D16" s="6">
+        <f t="shared" si="0"/>
+        <v>98100</v>
+      </c>
+      <c r="E16" t="s">
+        <v>22</v>
+      </c>
+      <c r="F16" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="7"/>

</xml_diff>

<commit_message>
update 12.1 10 2021
</commit_message>
<xml_diff>
--- a/rekap data uang kas kecil - asrama.xlsx
+++ b/rekap data uang kas kecil - asrama.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yofandi Riki Winata\Documents\yofandi\rekap data - uang galon, parkir, bumbu asrama\uangasrama\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25E2A502-7305-4B37-B81A-A1A4373D4A81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47D67CFB-E2C4-4BA2-850B-8CD59A7805C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{C456B771-9DF8-4725-AC5F-E2624C050843}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="32">
   <si>
     <t>Kas Kecil - Asrama STTHF</t>
   </si>
@@ -104,6 +104,30 @@
   </si>
   <si>
     <t>yofandi</t>
+  </si>
+  <si>
+    <t>uang beli ladaku, minyak, sabun colek, gula</t>
+  </si>
+  <si>
+    <t>uang beli galon (5 galon)</t>
+  </si>
+  <si>
+    <t>uang beli sirup cocopandan 2 botol &amp; nata de coco 2 bungkus di super indo</t>
+  </si>
+  <si>
+    <t>uang beli es batu 3 bungkus</t>
+  </si>
+  <si>
+    <t>uang parkir &amp; beli blewah 2 buah</t>
+  </si>
+  <si>
+    <t>uang masuk roku rungkut megah raya (paket indogrosir atas nama ce nanda)</t>
+  </si>
+  <si>
+    <t>uang beli galon (9 galon)</t>
+  </si>
+  <si>
+    <t>no</t>
   </si>
 </sst>
 </file>
@@ -518,32 +542,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1137C53-0063-4FE4-9637-7E05AFF16C56}">
-  <dimension ref="A1:N74"/>
+  <dimension ref="A1:O76"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="93" zoomScaleNormal="93" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9:A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="34.7109375" style="5" customWidth="1"/>
-    <col min="2" max="2" width="31.42578125" customWidth="1"/>
-    <col min="3" max="3" width="33.85546875" customWidth="1"/>
-    <col min="4" max="4" width="27.85546875" customWidth="1"/>
-    <col min="5" max="5" width="44.5703125" customWidth="1"/>
-    <col min="6" max="6" width="29.28515625" customWidth="1"/>
+    <col min="2" max="2" width="34.7109375" style="5" customWidth="1"/>
+    <col min="3" max="3" width="31.42578125" customWidth="1"/>
+    <col min="4" max="4" width="33.85546875" customWidth="1"/>
+    <col min="5" max="5" width="27.85546875" customWidth="1"/>
+    <col min="6" max="6" width="44.5703125" customWidth="1"/>
+    <col min="7" max="7" width="29.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="8"/>
+    <row r="1" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="8" t="s">
+        <v>0</v>
+      </c>
       <c r="C1" s="8"/>
       <c r="D1" s="8"/>
       <c r="E1" s="8"/>
       <c r="F1" s="8"/>
-      <c r="G1" s="2"/>
+      <c r="G1" s="8"/>
       <c r="H1" s="2"/>
       <c r="I1" s="2"/>
       <c r="J1" s="2"/>
@@ -551,15 +574,15 @@
       <c r="L1" s="2"/>
       <c r="M1" s="2"/>
       <c r="N1" s="2"/>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2" s="8"/>
+      <c r="O1" s="2"/>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B2" s="8"/>
       <c r="C2" s="8"/>
       <c r="D2" s="8"/>
       <c r="E2" s="8"/>
       <c r="F2" s="8"/>
-      <c r="G2" s="2"/>
+      <c r="G2" s="8"/>
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
       <c r="J2" s="2"/>
@@ -567,15 +590,15 @@
       <c r="L2" s="2"/>
       <c r="M2" s="2"/>
       <c r="N2" s="2"/>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A3" s="8"/>
+      <c r="O2" s="2"/>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B3" s="8"/>
       <c r="C3" s="8"/>
       <c r="D3" s="8"/>
       <c r="E3" s="8"/>
       <c r="F3" s="8"/>
-      <c r="G3" s="2"/>
+      <c r="G3" s="8"/>
       <c r="H3" s="2"/>
       <c r="I3" s="2"/>
       <c r="J3" s="2"/>
@@ -583,15 +606,15 @@
       <c r="L3" s="2"/>
       <c r="M3" s="2"/>
       <c r="N3" s="2"/>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A4" s="8"/>
+      <c r="O3" s="2"/>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B4" s="8"/>
       <c r="C4" s="8"/>
       <c r="D4" s="8"/>
       <c r="E4" s="8"/>
       <c r="F4" s="8"/>
-      <c r="G4" s="2"/>
+      <c r="G4" s="8"/>
       <c r="H4" s="2"/>
       <c r="I4" s="2"/>
       <c r="J4" s="2"/>
@@ -599,17 +622,17 @@
       <c r="L4" s="2"/>
       <c r="M4" s="2"/>
       <c r="N4" s="2"/>
-    </row>
-    <row r="5" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="9" t="s">
+      <c r="O4" s="2"/>
+    </row>
+    <row r="5" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="9"/>
       <c r="C5" s="9"/>
       <c r="D5" s="9"/>
       <c r="E5" s="9"/>
       <c r="F5" s="9"/>
-      <c r="G5" s="3"/>
+      <c r="G5" s="9"/>
       <c r="H5" s="3"/>
       <c r="I5" s="3"/>
       <c r="J5" s="3"/>
@@ -617,15 +640,15 @@
       <c r="L5" s="3"/>
       <c r="M5" s="3"/>
       <c r="N5" s="3"/>
-    </row>
-    <row r="6" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="9"/>
+      <c r="O5" s="3"/>
+    </row>
+    <row r="6" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="9"/>
       <c r="C6" s="9"/>
       <c r="D6" s="9"/>
       <c r="E6" s="9"/>
       <c r="F6" s="9"/>
-      <c r="G6" s="3"/>
+      <c r="G6" s="9"/>
       <c r="H6" s="3"/>
       <c r="I6" s="3"/>
       <c r="J6" s="3"/>
@@ -633,430 +656,684 @@
       <c r="L6" s="3"/>
       <c r="M6" s="3"/>
       <c r="N6" s="3"/>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
+      <c r="O6" s="3"/>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B7" s="5" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:15" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A8" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B8" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="C8" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="D8" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="E8" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="F8" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="F8" s="1" t="s">
+      <c r="G8" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A9" s="7">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>1</v>
+      </c>
+      <c r="B9" s="7">
         <v>44473</v>
       </c>
-      <c r="B9" s="6">
+      <c r="C9" s="6">
         <v>500000</v>
       </c>
-      <c r="C9" s="6">
-        <v>0</v>
-      </c>
       <c r="D9" s="6">
-        <f>B9-C9</f>
+        <v>0</v>
+      </c>
+      <c r="E9" s="6">
+        <f>C9-D9</f>
         <v>500000</v>
       </c>
-      <c r="E9" t="s">
+      <c r="F9" t="s">
         <v>8</v>
       </c>
-      <c r="F9" t="s">
+      <c r="G9" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A10" s="7">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>2</v>
+      </c>
+      <c r="B10" s="7">
         <v>44474</v>
       </c>
-      <c r="B10" s="6">
-        <v>0</v>
-      </c>
       <c r="C10" s="6">
+        <v>0</v>
+      </c>
+      <c r="D10" s="6">
         <v>70500</v>
       </c>
-      <c r="D10" s="6">
-        <f>D9+B10-C10</f>
+      <c r="E10" s="6">
+        <f>E9+C10-D10</f>
         <v>429500</v>
       </c>
-      <c r="E10" t="s">
+      <c r="F10" t="s">
         <v>11</v>
       </c>
-      <c r="F10" t="s">
+      <c r="G10" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A11" s="7">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>3</v>
+      </c>
+      <c r="B11" s="7">
         <v>44475</v>
       </c>
-      <c r="B11" s="6">
-        <v>0</v>
-      </c>
       <c r="C11" s="6">
+        <v>0</v>
+      </c>
+      <c r="D11" s="6">
         <v>17500</v>
       </c>
-      <c r="D11" s="6">
-        <f t="shared" ref="D11:D16" si="0">D10+B11-C11</f>
+      <c r="E11" s="6">
+        <f t="shared" ref="E11:E19" si="0">E10+C11-D11</f>
         <v>412000</v>
       </c>
-      <c r="E11" t="s">
+      <c r="F11" t="s">
         <v>13</v>
       </c>
-      <c r="F11" t="s">
+      <c r="G11" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A12" s="7">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>4</v>
+      </c>
+      <c r="B12" s="7">
         <v>44475</v>
       </c>
-      <c r="B12" s="6">
-        <v>0</v>
-      </c>
       <c r="C12" s="6">
+        <v>0</v>
+      </c>
+      <c r="D12" s="6">
         <v>35700</v>
       </c>
-      <c r="D12" s="6">
+      <c r="E12" s="6">
         <f t="shared" si="0"/>
         <v>376300</v>
       </c>
-      <c r="E12" t="s">
+      <c r="F12" t="s">
         <v>15</v>
       </c>
-      <c r="F12" t="s">
+      <c r="G12" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A13" s="7">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>5</v>
+      </c>
+      <c r="B13" s="7">
         <v>44476</v>
       </c>
-      <c r="B13" s="6">
-        <v>0</v>
-      </c>
       <c r="C13" s="6">
+        <v>0</v>
+      </c>
+      <c r="D13" s="6">
         <v>154000</v>
       </c>
-      <c r="D13" s="6">
+      <c r="E13" s="6">
         <f t="shared" si="0"/>
         <v>222300</v>
       </c>
-      <c r="E13" t="s">
+      <c r="F13" t="s">
         <v>16</v>
       </c>
-      <c r="F13" t="s">
+      <c r="G13" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A14" s="7">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>6</v>
+      </c>
+      <c r="B14" s="7">
         <v>44476</v>
       </c>
-      <c r="B14" s="6">
-        <v>0</v>
-      </c>
       <c r="C14" s="6">
+        <v>0</v>
+      </c>
+      <c r="D14" s="6">
         <v>101200</v>
       </c>
-      <c r="D14" s="6">
+      <c r="E14" s="6">
         <f t="shared" si="0"/>
         <v>121100</v>
       </c>
-      <c r="E14" t="s">
+      <c r="F14" t="s">
         <v>18</v>
       </c>
-      <c r="F14" t="s">
+      <c r="G14" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A15" s="7">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>7</v>
+      </c>
+      <c r="B15" s="7">
         <v>44476</v>
       </c>
-      <c r="B15" s="6">
-        <v>0</v>
-      </c>
       <c r="C15" s="6">
+        <v>0</v>
+      </c>
+      <c r="D15" s="6">
         <v>13000</v>
       </c>
-      <c r="D15" s="6">
+      <c r="E15" s="6">
         <f t="shared" si="0"/>
         <v>108100</v>
       </c>
-      <c r="E15" t="s">
+      <c r="F15" t="s">
         <v>20</v>
       </c>
-      <c r="F15" t="s">
+      <c r="G15" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A16" s="7">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>8</v>
+      </c>
+      <c r="B16" s="7">
         <v>44477</v>
       </c>
-      <c r="B16" s="6">
-        <v>0</v>
-      </c>
       <c r="C16" s="6">
+        <v>0</v>
+      </c>
+      <c r="D16" s="6">
         <v>10000</v>
       </c>
-      <c r="D16" s="6">
+      <c r="E16" s="6">
         <f t="shared" si="0"/>
         <v>98100</v>
       </c>
-      <c r="E16" t="s">
+      <c r="F16" t="s">
         <v>22</v>
       </c>
-      <c r="F16" t="s">
+      <c r="G16" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="7"/>
-      <c r="B17" s="6"/>
-      <c r="C17" s="6"/>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="7"/>
-      <c r="B18" s="6"/>
-      <c r="C18" s="6"/>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="7"/>
-      <c r="B19" s="6"/>
-      <c r="C19" s="6"/>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="7"/>
-      <c r="B20" s="6"/>
-      <c r="C20" s="6"/>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="7"/>
-      <c r="B21" s="6"/>
-      <c r="C21" s="6"/>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="7"/>
-      <c r="B22" s="6"/>
-      <c r="C22" s="6"/>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="7"/>
-      <c r="B23" s="6"/>
-      <c r="C23" s="6"/>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="7"/>
-      <c r="B24" s="6"/>
-      <c r="C24" s="6"/>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="7"/>
-      <c r="B25" s="6"/>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>9</v>
+      </c>
+      <c r="B17" s="7">
+        <v>44480</v>
+      </c>
+      <c r="C17" s="6">
+        <v>0</v>
+      </c>
+      <c r="D17" s="6">
+        <v>79000</v>
+      </c>
+      <c r="E17" s="6">
+        <f t="shared" si="0"/>
+        <v>19100</v>
+      </c>
+      <c r="F17" t="s">
+        <v>24</v>
+      </c>
+      <c r="G17" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>10</v>
+      </c>
+      <c r="B18" s="7">
+        <v>44480</v>
+      </c>
+      <c r="C18" s="6">
+        <v>0</v>
+      </c>
+      <c r="D18" s="6">
+        <v>37500</v>
+      </c>
+      <c r="E18" s="6">
+        <f t="shared" si="0"/>
+        <v>-18400</v>
+      </c>
+      <c r="F18" t="s">
+        <v>25</v>
+      </c>
+      <c r="G18" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>11</v>
+      </c>
+      <c r="B19" s="7">
+        <v>44481</v>
+      </c>
+      <c r="C19" s="6">
+        <v>500000</v>
+      </c>
+      <c r="D19" s="6">
+        <v>0</v>
+      </c>
+      <c r="E19" s="6">
+        <f>E18+C19-D19</f>
+        <v>481600</v>
+      </c>
+      <c r="F19" t="s">
+        <v>8</v>
+      </c>
+      <c r="G19" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>12</v>
+      </c>
+      <c r="B20" s="7">
+        <v>44481</v>
+      </c>
+      <c r="C20" s="6">
+        <v>0</v>
+      </c>
+      <c r="D20" s="6">
+        <v>67400</v>
+      </c>
+      <c r="E20" s="6">
+        <f t="shared" ref="E20:E41" si="1">E19+C20-D20</f>
+        <v>414200</v>
+      </c>
+      <c r="F20" t="s">
+        <v>26</v>
+      </c>
+      <c r="G20" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>13</v>
+      </c>
+      <c r="B21" s="7">
+        <v>44481</v>
+      </c>
+      <c r="C21" s="6">
+        <v>0</v>
+      </c>
+      <c r="D21" s="6">
+        <v>23000</v>
+      </c>
+      <c r="E21" s="6">
+        <f t="shared" si="1"/>
+        <v>391200</v>
+      </c>
+      <c r="F21" t="s">
+        <v>28</v>
+      </c>
+      <c r="G21" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>14</v>
+      </c>
+      <c r="B22" s="7">
+        <v>44481</v>
+      </c>
+      <c r="C22" s="6">
+        <v>0</v>
+      </c>
+      <c r="D22" s="6">
+        <v>15000</v>
+      </c>
+      <c r="E22" s="6">
+        <f t="shared" si="1"/>
+        <v>376200</v>
+      </c>
+      <c r="F22" t="s">
+        <v>27</v>
+      </c>
+      <c r="G22" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>15</v>
+      </c>
+      <c r="B23" s="7">
+        <v>44481</v>
+      </c>
+      <c r="C23" s="6">
+        <v>0</v>
+      </c>
+      <c r="D23" s="6">
+        <v>6000</v>
+      </c>
+      <c r="E23" s="6">
+        <f t="shared" si="1"/>
+        <v>370200</v>
+      </c>
+      <c r="F23" t="s">
+        <v>29</v>
+      </c>
+      <c r="G23" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>16</v>
+      </c>
+      <c r="B24" s="7">
+        <v>44481</v>
+      </c>
+      <c r="C24" s="6">
+        <v>0</v>
+      </c>
+      <c r="D24" s="6">
+        <v>70500</v>
+      </c>
+      <c r="E24" s="6">
+        <f t="shared" si="1"/>
+        <v>299700</v>
+      </c>
+      <c r="F24" t="s">
+        <v>30</v>
+      </c>
+      <c r="G24" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B25" s="7"/>
       <c r="C25" s="6"/>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="7"/>
-      <c r="B26" s="6"/>
+      <c r="D25" s="6"/>
+      <c r="E25" s="6">
+        <f t="shared" si="1"/>
+        <v>299700</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B26" s="7"/>
       <c r="C26" s="6"/>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="7"/>
-      <c r="B27" s="6"/>
+      <c r="D26" s="6"/>
+      <c r="E26" s="6">
+        <f t="shared" si="1"/>
+        <v>299700</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B27" s="7"/>
       <c r="C27" s="6"/>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="7"/>
-      <c r="B28" s="6"/>
+      <c r="D27" s="6"/>
+      <c r="E27" s="6">
+        <f t="shared" si="1"/>
+        <v>299700</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B28" s="7"/>
       <c r="C28" s="6"/>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" s="7"/>
-      <c r="B29" s="6"/>
+      <c r="D28" s="6"/>
+      <c r="E28" s="6">
+        <f t="shared" si="1"/>
+        <v>299700</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B29" s="7"/>
       <c r="C29" s="6"/>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" s="7"/>
-      <c r="B30" s="6"/>
+      <c r="D29" s="6"/>
+      <c r="E29" s="6">
+        <f t="shared" si="1"/>
+        <v>299700</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B30" s="7"/>
       <c r="C30" s="6"/>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" s="7"/>
-      <c r="B31" s="6"/>
+      <c r="D30" s="6"/>
+      <c r="E30" s="6">
+        <f t="shared" si="1"/>
+        <v>299700</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B31" s="7"/>
       <c r="C31" s="6"/>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" s="7"/>
-      <c r="B32" s="6"/>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" s="7"/>
-      <c r="B33" s="6"/>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" s="7"/>
-      <c r="B34" s="6"/>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" s="7"/>
-      <c r="B35" s="6"/>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" s="7"/>
-      <c r="B36" s="6"/>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" s="7"/>
-      <c r="B37" s="6"/>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38" s="7"/>
-      <c r="B38" s="6"/>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39" s="7"/>
-      <c r="B39" s="6"/>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A40" s="7"/>
-      <c r="B40" s="6"/>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A41" s="7"/>
-      <c r="B41" s="6"/>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A42" s="7"/>
-      <c r="B42" s="6"/>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A43" s="7"/>
-      <c r="B43" s="6"/>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A44" s="7"/>
-      <c r="B44" s="6"/>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A45" s="7"/>
-      <c r="B45" s="6"/>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A46" s="7"/>
-      <c r="B46" s="6"/>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A47" s="7"/>
-      <c r="B47" s="6"/>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A48" s="7"/>
-      <c r="B48" s="6"/>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A49" s="7"/>
-      <c r="B49" s="6"/>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A50" s="7"/>
-      <c r="B50" s="6"/>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A51" s="7"/>
-      <c r="B51" s="6"/>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A52" s="7"/>
-      <c r="B52" s="6"/>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A53" s="7"/>
-      <c r="B53" s="6"/>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A54" s="7"/>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A55" s="7"/>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A56" s="7"/>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A57" s="7"/>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A58" s="7"/>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A59" s="7"/>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A60" s="7"/>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A61" s="7"/>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A62" s="7"/>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A63" s="7"/>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A64" s="7"/>
-    </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A65" s="7"/>
-    </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A66" s="7"/>
-    </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A67" s="7"/>
-    </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A68" s="7"/>
-    </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A69" s="7"/>
-    </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A70" s="7"/>
-    </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A71" s="7"/>
-    </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A72" s="7"/>
-    </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A73" s="7"/>
-    </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A74" s="7"/>
+      <c r="D31" s="6"/>
+      <c r="E31" s="6">
+        <f t="shared" si="1"/>
+        <v>299700</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B32" s="7"/>
+      <c r="C32" s="6"/>
+      <c r="E32" s="6">
+        <f t="shared" si="1"/>
+        <v>299700</v>
+      </c>
+    </row>
+    <row r="33" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B33" s="7"/>
+      <c r="C33" s="6"/>
+      <c r="E33" s="6">
+        <f t="shared" si="1"/>
+        <v>299700</v>
+      </c>
+    </row>
+    <row r="34" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B34" s="7"/>
+      <c r="C34" s="6"/>
+      <c r="E34" s="6">
+        <f t="shared" si="1"/>
+        <v>299700</v>
+      </c>
+    </row>
+    <row r="35" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B35" s="7"/>
+      <c r="C35" s="6"/>
+      <c r="E35" s="6">
+        <f t="shared" si="1"/>
+        <v>299700</v>
+      </c>
+    </row>
+    <row r="36" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B36" s="7"/>
+      <c r="C36" s="6"/>
+      <c r="E36" s="6">
+        <f t="shared" si="1"/>
+        <v>299700</v>
+      </c>
+    </row>
+    <row r="37" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B37" s="7"/>
+      <c r="C37" s="6"/>
+      <c r="E37" s="6">
+        <f t="shared" si="1"/>
+        <v>299700</v>
+      </c>
+    </row>
+    <row r="38" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B38" s="7"/>
+      <c r="C38" s="6"/>
+      <c r="E38" s="6">
+        <f t="shared" si="1"/>
+        <v>299700</v>
+      </c>
+    </row>
+    <row r="39" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B39" s="7"/>
+      <c r="C39" s="6"/>
+      <c r="E39" s="6">
+        <f t="shared" si="1"/>
+        <v>299700</v>
+      </c>
+    </row>
+    <row r="40" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B40" s="7"/>
+      <c r="C40" s="6"/>
+      <c r="E40" s="6">
+        <f t="shared" si="1"/>
+        <v>299700</v>
+      </c>
+    </row>
+    <row r="41" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B41" s="7"/>
+      <c r="C41" s="6"/>
+      <c r="E41" s="6">
+        <f t="shared" si="1"/>
+        <v>299700</v>
+      </c>
+    </row>
+    <row r="42" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B42" s="7"/>
+      <c r="C42" s="6"/>
+    </row>
+    <row r="43" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B43" s="7"/>
+      <c r="C43" s="6"/>
+    </row>
+    <row r="44" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B44" s="7"/>
+      <c r="C44" s="6"/>
+    </row>
+    <row r="45" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B45" s="7"/>
+      <c r="C45" s="6"/>
+    </row>
+    <row r="46" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B46" s="7"/>
+      <c r="C46" s="6"/>
+    </row>
+    <row r="47" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B47" s="7"/>
+      <c r="C47" s="6"/>
+    </row>
+    <row r="48" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B48" s="7"/>
+      <c r="C48" s="6"/>
+    </row>
+    <row r="49" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B49" s="7"/>
+      <c r="C49" s="6"/>
+    </row>
+    <row r="50" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B50" s="7"/>
+      <c r="C50" s="6"/>
+    </row>
+    <row r="51" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B51" s="7"/>
+      <c r="C51" s="6"/>
+    </row>
+    <row r="52" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B52" s="7"/>
+      <c r="C52" s="6"/>
+    </row>
+    <row r="53" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B53" s="7"/>
+      <c r="C53" s="6"/>
+    </row>
+    <row r="54" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B54" s="7"/>
+    </row>
+    <row r="55" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B55" s="7"/>
+    </row>
+    <row r="56" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B56" s="7"/>
+    </row>
+    <row r="57" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B57" s="7"/>
+    </row>
+    <row r="58" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B58" s="7"/>
+    </row>
+    <row r="59" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B59" s="7"/>
+    </row>
+    <row r="60" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B60" s="7"/>
+    </row>
+    <row r="61" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B61" s="7"/>
+    </row>
+    <row r="62" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B62" s="7"/>
+    </row>
+    <row r="63" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B63" s="7"/>
+    </row>
+    <row r="64" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B64" s="7"/>
+    </row>
+    <row r="65" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B65" s="7"/>
+    </row>
+    <row r="66" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B66" s="7"/>
+    </row>
+    <row r="67" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B67" s="7"/>
+    </row>
+    <row r="68" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B68" s="7"/>
+    </row>
+    <row r="69" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B69" s="7"/>
+    </row>
+    <row r="70" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B70" s="7"/>
+    </row>
+    <row r="71" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B71" s="7"/>
+    </row>
+    <row r="72" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B72" s="7"/>
+    </row>
+    <row r="73" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B73" s="7"/>
+    </row>
+    <row r="74" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B74" s="7"/>
+    </row>
+    <row r="75" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B75" s="7"/>
+    </row>
+    <row r="76" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B76" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A1:F4"/>
-    <mergeCell ref="A5:F6"/>
+    <mergeCell ref="B1:G4"/>
+    <mergeCell ref="B5:G6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
update 16 10 2021
</commit_message>
<xml_diff>
--- a/rekap data uang kas kecil - asrama.xlsx
+++ b/rekap data uang kas kecil - asrama.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yofandi Riki Winata\Documents\yofandi\rekap data - uang galon, parkir, bumbu asrama\uangasrama\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47D67CFB-E2C4-4BA2-850B-8CD59A7805C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{332CC5F0-247C-4CA5-90EF-1AED64A8C940}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{C456B771-9DF8-4725-AC5F-E2624C050843}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="39">
   <si>
     <t>Kas Kecil - Asrama STTHF</t>
   </si>
@@ -128,6 +128,27 @@
   </si>
   <si>
     <t>no</t>
+  </si>
+  <si>
+    <t>uang beli tespan, voltmeter sama lem G</t>
+  </si>
+  <si>
+    <t>Saferius sama Hosea</t>
+  </si>
+  <si>
+    <t>uang beli tabung gas 3 kg (2 tabung)</t>
+  </si>
+  <si>
+    <t>jhonan sama peter</t>
+  </si>
+  <si>
+    <t>uang beli DHS machine head (puteran gitar)</t>
+  </si>
+  <si>
+    <t>Saferius sama tondo</t>
+  </si>
+  <si>
+    <t>uang parkir</t>
   </si>
 </sst>
 </file>
@@ -544,8 +565,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1137C53-0063-4FE4-9637-7E05AFF16C56}">
   <dimension ref="A1:O76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="93" zoomScaleNormal="93" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9:A24"/>
+    <sheetView tabSelected="1" topLeftCell="B6" zoomScale="90" zoomScaleNormal="90" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -748,7 +769,7 @@
         <v>17500</v>
       </c>
       <c r="E11" s="6">
-        <f t="shared" ref="E11:E19" si="0">E10+C11-D11</f>
+        <f t="shared" ref="E11:E18" si="0">E10+C11-D11</f>
         <v>412000</v>
       </c>
       <c r="F11" t="s">
@@ -964,7 +985,7 @@
         <v>67400</v>
       </c>
       <c r="E20" s="6">
-        <f t="shared" ref="E20:E41" si="1">E19+C20-D20</f>
+        <f t="shared" ref="E20:E35" si="1">E19+C20-D20</f>
         <v>414200</v>
       </c>
       <c r="F20" t="s">
@@ -1027,7 +1048,7 @@
         <v>15</v>
       </c>
       <c r="B23" s="7">
-        <v>44481</v>
+        <v>44482</v>
       </c>
       <c r="C23" s="6">
         <v>0</v>
@@ -1051,7 +1072,7 @@
         <v>16</v>
       </c>
       <c r="B24" s="7">
-        <v>44481</v>
+        <v>44482</v>
       </c>
       <c r="C24" s="6">
         <v>0</v>
@@ -1071,57 +1092,147 @@
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B25" s="7"/>
-      <c r="C25" s="6"/>
-      <c r="D25" s="6"/>
+      <c r="A25">
+        <v>17</v>
+      </c>
+      <c r="B25" s="7">
+        <v>44483</v>
+      </c>
+      <c r="C25" s="6">
+        <v>0</v>
+      </c>
+      <c r="D25" s="6">
+        <v>84500</v>
+      </c>
       <c r="E25" s="6">
         <f t="shared" si="1"/>
-        <v>299700</v>
+        <v>215200</v>
+      </c>
+      <c r="F25" t="s">
+        <v>32</v>
+      </c>
+      <c r="G25" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B26" s="7"/>
-      <c r="C26" s="6"/>
-      <c r="D26" s="6"/>
+      <c r="A26">
+        <v>18</v>
+      </c>
+      <c r="B26" s="7">
+        <v>44485</v>
+      </c>
+      <c r="C26" s="6">
+        <v>0</v>
+      </c>
+      <c r="D26" s="6">
+        <v>32000</v>
+      </c>
       <c r="E26" s="6">
         <f t="shared" si="1"/>
-        <v>299700</v>
+        <v>183200</v>
+      </c>
+      <c r="F26" t="s">
+        <v>34</v>
+      </c>
+      <c r="G26" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B27" s="7"/>
-      <c r="C27" s="6"/>
-      <c r="D27" s="6"/>
+      <c r="A27">
+        <v>19</v>
+      </c>
+      <c r="B27" s="7">
+        <v>44485</v>
+      </c>
+      <c r="C27" s="6">
+        <v>0</v>
+      </c>
+      <c r="D27" s="6">
+        <v>31700</v>
+      </c>
       <c r="E27" s="6">
         <f t="shared" si="1"/>
-        <v>299700</v>
+        <v>151500</v>
+      </c>
+      <c r="F27" t="s">
+        <v>15</v>
+      </c>
+      <c r="G27" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B28" s="7"/>
-      <c r="C28" s="6"/>
-      <c r="D28" s="6"/>
+      <c r="A28">
+        <v>20</v>
+      </c>
+      <c r="B28" s="7">
+        <v>44485</v>
+      </c>
+      <c r="C28" s="6">
+        <v>0</v>
+      </c>
+      <c r="D28" s="6">
+        <v>55000</v>
+      </c>
       <c r="E28" s="6">
         <f t="shared" si="1"/>
-        <v>299700</v>
+        <v>96500</v>
+      </c>
+      <c r="F28" t="s">
+        <v>36</v>
+      </c>
+      <c r="G28" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B29" s="7"/>
-      <c r="C29" s="6"/>
-      <c r="D29" s="6"/>
+      <c r="A29">
+        <v>21</v>
+      </c>
+      <c r="B29" s="7">
+        <v>44485</v>
+      </c>
+      <c r="C29" s="6">
+        <v>0</v>
+      </c>
+      <c r="D29" s="6">
+        <v>10000</v>
+      </c>
       <c r="E29" s="6">
         <f t="shared" si="1"/>
-        <v>299700</v>
+        <v>86500</v>
+      </c>
+      <c r="F29" t="s">
+        <v>22</v>
+      </c>
+      <c r="G29" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B30" s="7"/>
-      <c r="C30" s="6"/>
-      <c r="D30" s="6"/>
+      <c r="A30">
+        <v>22</v>
+      </c>
+      <c r="B30" s="7">
+        <v>44485</v>
+      </c>
+      <c r="C30" s="6">
+        <v>0</v>
+      </c>
+      <c r="D30" s="6">
+        <v>2000</v>
+      </c>
       <c r="E30" s="6">
         <f t="shared" si="1"/>
-        <v>299700</v>
+        <v>84500</v>
+      </c>
+      <c r="F30" t="s">
+        <v>38</v>
+      </c>
+      <c r="G30" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
@@ -1130,7 +1241,7 @@
       <c r="D31" s="6"/>
       <c r="E31" s="6">
         <f t="shared" si="1"/>
-        <v>299700</v>
+        <v>84500</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
@@ -1138,7 +1249,7 @@
       <c r="C32" s="6"/>
       <c r="E32" s="6">
         <f t="shared" si="1"/>
-        <v>299700</v>
+        <v>84500</v>
       </c>
     </row>
     <row r="33" spans="2:5" x14ac:dyDescent="0.25">
@@ -1146,7 +1257,7 @@
       <c r="C33" s="6"/>
       <c r="E33" s="6">
         <f t="shared" si="1"/>
-        <v>299700</v>
+        <v>84500</v>
       </c>
     </row>
     <row r="34" spans="2:5" x14ac:dyDescent="0.25">
@@ -1154,7 +1265,7 @@
       <c r="C34" s="6"/>
       <c r="E34" s="6">
         <f t="shared" si="1"/>
-        <v>299700</v>
+        <v>84500</v>
       </c>
     </row>
     <row r="35" spans="2:5" x14ac:dyDescent="0.25">
@@ -1162,56 +1273,38 @@
       <c r="C35" s="6"/>
       <c r="E35" s="6">
         <f t="shared" si="1"/>
-        <v>299700</v>
+        <v>84500</v>
       </c>
     </row>
     <row r="36" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B36" s="7"/>
       <c r="C36" s="6"/>
-      <c r="E36" s="6">
-        <f t="shared" si="1"/>
-        <v>299700</v>
-      </c>
+      <c r="E36" s="6"/>
     </row>
     <row r="37" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B37" s="7"/>
       <c r="C37" s="6"/>
-      <c r="E37" s="6">
-        <f t="shared" si="1"/>
-        <v>299700</v>
-      </c>
+      <c r="E37" s="6"/>
     </row>
     <row r="38" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B38" s="7"/>
       <c r="C38" s="6"/>
-      <c r="E38" s="6">
-        <f t="shared" si="1"/>
-        <v>299700</v>
-      </c>
+      <c r="E38" s="6"/>
     </row>
     <row r="39" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B39" s="7"/>
       <c r="C39" s="6"/>
-      <c r="E39" s="6">
-        <f t="shared" si="1"/>
-        <v>299700</v>
-      </c>
+      <c r="E39" s="6"/>
     </row>
     <row r="40" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B40" s="7"/>
       <c r="C40" s="6"/>
-      <c r="E40" s="6">
-        <f t="shared" si="1"/>
-        <v>299700</v>
-      </c>
+      <c r="E40" s="6"/>
     </row>
     <row r="41" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B41" s="7"/>
       <c r="C41" s="6"/>
-      <c r="E41" s="6">
-        <f t="shared" si="1"/>
-        <v>299700</v>
-      </c>
+      <c r="E41" s="6"/>
     </row>
     <row r="42" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B42" s="7"/>

</xml_diff>

<commit_message>
update 21 10 2021
</commit_message>
<xml_diff>
--- a/rekap data uang kas kecil - asrama.xlsx
+++ b/rekap data uang kas kecil - asrama.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yofandi Riki Winata\Documents\yofandi\rekap data - uang galon, parkir, bumbu asrama\uangasrama\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{332CC5F0-247C-4CA5-90EF-1AED64A8C940}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCCFD7AA-1353-47E6-9DC2-E4C27B690195}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{C456B771-9DF8-4725-AC5F-E2624C050843}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="48">
   <si>
     <t>Kas Kecil - Asrama STTHF</t>
   </si>
@@ -149,6 +149,33 @@
   </si>
   <si>
     <t>uang parkir</t>
+  </si>
+  <si>
+    <t>uang beli kran tandon</t>
+  </si>
+  <si>
+    <t>peter sama valen</t>
+  </si>
+  <si>
+    <t>uang galon aqua (10)</t>
+  </si>
+  <si>
+    <t>valen sama hosea</t>
+  </si>
+  <si>
+    <t>uang beli nata de coco</t>
+  </si>
+  <si>
+    <t>yofandi sama valen</t>
+  </si>
+  <si>
+    <t>uang beli semangka, melon, isi ban motor, parkir</t>
+  </si>
+  <si>
+    <t>uang beli bensin pertamax avanza</t>
+  </si>
+  <si>
+    <t>uang beli sate ayam 100 tusuk</t>
   </si>
 </sst>
 </file>
@@ -565,13 +592,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1137C53-0063-4FE4-9637-7E05AFF16C56}">
   <dimension ref="A1:O76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B6" zoomScale="90" zoomScaleNormal="90" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="D31" sqref="D31"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="80" zoomScaleNormal="80" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="E38" sqref="E38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="34.7109375" style="5" customWidth="1"/>
+    <col min="2" max="2" width="23.28515625" style="5" customWidth="1"/>
     <col min="3" max="3" width="31.42578125" customWidth="1"/>
     <col min="4" max="4" width="33.85546875" customWidth="1"/>
     <col min="5" max="5" width="27.85546875" customWidth="1"/>
@@ -985,7 +1012,7 @@
         <v>67400</v>
       </c>
       <c r="E20" s="6">
-        <f t="shared" ref="E20:E35" si="1">E19+C20-D20</f>
+        <f t="shared" ref="E20:E40" si="1">E19+C20-D20</f>
         <v>414200</v>
       </c>
       <c r="F20" t="s">
@@ -1236,101 +1263,259 @@
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B31" s="7"/>
-      <c r="C31" s="6"/>
-      <c r="D31" s="6"/>
+      <c r="A31">
+        <v>23</v>
+      </c>
+      <c r="B31" s="7">
+        <v>44486</v>
+      </c>
+      <c r="C31" s="6">
+        <v>0</v>
+      </c>
+      <c r="D31" s="6">
+        <v>110000</v>
+      </c>
       <c r="E31" s="6">
         <f t="shared" si="1"/>
-        <v>84500</v>
+        <v>-25500</v>
+      </c>
+      <c r="F31" t="s">
+        <v>39</v>
+      </c>
+      <c r="G31" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B32" s="7"/>
-      <c r="C32" s="6"/>
+      <c r="A32">
+        <v>24</v>
+      </c>
+      <c r="B32" s="7">
+        <v>44487</v>
+      </c>
+      <c r="C32" s="6">
+        <v>500000</v>
+      </c>
+      <c r="D32" s="6">
+        <v>0</v>
+      </c>
       <c r="E32" s="6">
         <f t="shared" si="1"/>
-        <v>84500</v>
-      </c>
-    </row>
-    <row r="33" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B33" s="7"/>
-      <c r="C33" s="6"/>
+        <v>474500</v>
+      </c>
+      <c r="F32" t="s">
+        <v>8</v>
+      </c>
+      <c r="G32" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>25</v>
+      </c>
+      <c r="B33" s="7">
+        <v>44487</v>
+      </c>
+      <c r="C33" s="6">
+        <v>0</v>
+      </c>
+      <c r="D33" s="6">
+        <v>32900</v>
+      </c>
       <c r="E33" s="6">
         <f t="shared" si="1"/>
-        <v>84500</v>
-      </c>
-    </row>
-    <row r="34" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B34" s="7"/>
-      <c r="C34" s="6"/>
+        <v>441600</v>
+      </c>
+      <c r="F33" t="s">
+        <v>15</v>
+      </c>
+      <c r="G33" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>26</v>
+      </c>
+      <c r="B34" s="7">
+        <v>44488</v>
+      </c>
+      <c r="C34" s="6">
+        <v>0</v>
+      </c>
+      <c r="D34" s="6">
+        <v>78000</v>
+      </c>
       <c r="E34" s="6">
         <f t="shared" si="1"/>
-        <v>84500</v>
-      </c>
-    </row>
-    <row r="35" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B35" s="7"/>
-      <c r="C35" s="6"/>
+        <v>363600</v>
+      </c>
+      <c r="F34" t="s">
+        <v>41</v>
+      </c>
+      <c r="G34" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>27</v>
+      </c>
+      <c r="B35" s="7">
+        <v>44488</v>
+      </c>
+      <c r="C35" s="6">
+        <v>0</v>
+      </c>
+      <c r="D35" s="6">
+        <v>10000</v>
+      </c>
       <c r="E35" s="6">
         <f t="shared" si="1"/>
-        <v>84500</v>
-      </c>
-    </row>
-    <row r="36" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B36" s="7"/>
-      <c r="C36" s="6"/>
-      <c r="E36" s="6"/>
-    </row>
-    <row r="37" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B37" s="7"/>
-      <c r="C37" s="6"/>
-      <c r="E37" s="6"/>
-    </row>
-    <row r="38" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B38" s="7"/>
-      <c r="C38" s="6"/>
-      <c r="E38" s="6"/>
-    </row>
-    <row r="39" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B39" s="7"/>
-      <c r="C39" s="6"/>
-      <c r="E39" s="6"/>
-    </row>
-    <row r="40" spans="2:5" x14ac:dyDescent="0.25">
+        <v>353600</v>
+      </c>
+      <c r="F35" t="s">
+        <v>22</v>
+      </c>
+      <c r="G35" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>28</v>
+      </c>
+      <c r="B36" s="7">
+        <v>44490</v>
+      </c>
+      <c r="C36" s="6">
+        <v>0</v>
+      </c>
+      <c r="D36" s="6">
+        <v>33000</v>
+      </c>
+      <c r="E36" s="6">
+        <f t="shared" si="1"/>
+        <v>320600</v>
+      </c>
+      <c r="F36" t="s">
+        <v>43</v>
+      </c>
+      <c r="G36" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>29</v>
+      </c>
+      <c r="B37" s="7">
+        <v>44490</v>
+      </c>
+      <c r="C37" s="6">
+        <v>0</v>
+      </c>
+      <c r="D37" s="6">
+        <v>69000</v>
+      </c>
+      <c r="E37" s="6">
+        <f t="shared" si="1"/>
+        <v>251600</v>
+      </c>
+      <c r="F37" t="s">
+        <v>45</v>
+      </c>
+      <c r="G37" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>30</v>
+      </c>
+      <c r="B38" s="7">
+        <v>44490</v>
+      </c>
+      <c r="C38" s="6">
+        <v>0</v>
+      </c>
+      <c r="D38" s="6">
+        <v>100000</v>
+      </c>
+      <c r="E38" s="6">
+        <f t="shared" si="1"/>
+        <v>151600</v>
+      </c>
+      <c r="F38" t="s">
+        <v>46</v>
+      </c>
+      <c r="G38" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>31</v>
+      </c>
+      <c r="B39" s="7">
+        <v>44490</v>
+      </c>
+      <c r="C39" s="6">
+        <v>0</v>
+      </c>
+      <c r="D39" s="6">
+        <v>117000</v>
+      </c>
+      <c r="E39" s="6">
+        <f t="shared" si="1"/>
+        <v>34600</v>
+      </c>
+      <c r="F39" t="s">
+        <v>47</v>
+      </c>
+      <c r="G39" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B40" s="7"/>
       <c r="C40" s="6"/>
-      <c r="E40" s="6"/>
-    </row>
-    <row r="41" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E40" s="6">
+        <f t="shared" si="1"/>
+        <v>34600</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B41" s="7"/>
       <c r="C41" s="6"/>
       <c r="E41" s="6"/>
     </row>
-    <row r="42" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B42" s="7"/>
       <c r="C42" s="6"/>
     </row>
-    <row r="43" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B43" s="7"/>
       <c r="C43" s="6"/>
     </row>
-    <row r="44" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B44" s="7"/>
       <c r="C44" s="6"/>
     </row>
-    <row r="45" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B45" s="7"/>
       <c r="C45" s="6"/>
     </row>
-    <row r="46" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B46" s="7"/>
       <c r="C46" s="6"/>
     </row>
-    <row r="47" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B47" s="7"/>
       <c r="C47" s="6"/>
     </row>
-    <row r="48" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B48" s="7"/>
       <c r="C48" s="6"/>
     </row>

</xml_diff>

<commit_message>
update 05 11 2021
</commit_message>
<xml_diff>
--- a/rekap data uang kas kecil - asrama.xlsx
+++ b/rekap data uang kas kecil - asrama.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yofandi Riki Winata\Documents\yofandi\rekap data - uang galon, parkir, bumbu asrama\uangasrama\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCCFD7AA-1353-47E6-9DC2-E4C27B690195}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1B2D0FB-8EC7-475C-BB6F-3CA414B9FD8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{C456B771-9DF8-4725-AC5F-E2624C050843}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" activeTab="1" xr2:uid="{C456B771-9DF8-4725-AC5F-E2624C050843}"/>
   </bookViews>
   <sheets>
     <sheet name="Oktober" sheetId="1" r:id="rId1"/>
+    <sheet name="November" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="79">
   <si>
     <t>Kas Kecil - Asrama STTHF</t>
   </si>
@@ -176,18 +177,112 @@
   </si>
   <si>
     <t>uang beli sate ayam 100 tusuk</t>
+  </si>
+  <si>
+    <t>uang beli pongstan 500mg</t>
+  </si>
+  <si>
+    <t>hosea</t>
+  </si>
+  <si>
+    <t>uamg masuk dari Ce Nanda, uang kas kecil asrama</t>
+  </si>
+  <si>
+    <t>uang bensin pertamax motor</t>
+  </si>
+  <si>
+    <t>uang beli es batu 2 bungkus</t>
+  </si>
+  <si>
+    <t>uang beli sirup cocopandan 2 botol &amp; nata de coco 2 bungkus &amp; gula 2 bungkus di super indo</t>
+  </si>
+  <si>
+    <t>uang bensin perlite motot</t>
+  </si>
+  <si>
+    <t>saferius</t>
+  </si>
+  <si>
+    <t>uang beli t.bombong</t>
+  </si>
+  <si>
+    <t>uang beli gas elpiji 3kg (3buah)</t>
+  </si>
+  <si>
+    <t>uang bensin avanza untuk njemput dosen</t>
+  </si>
+  <si>
+    <t>uang beli galon aqua (10galon)</t>
+  </si>
+  <si>
+    <t>uang beli es batu (2kantong)</t>
+  </si>
+  <si>
+    <t>uang masuk ruko rich palace</t>
+  </si>
+  <si>
+    <t>uang masuk ruko rungkut megah raya (grab cece nanda)</t>
+  </si>
+  <si>
+    <t>uang beli pertalite motor</t>
+  </si>
+  <si>
+    <t>saferius sama peter</t>
+  </si>
+  <si>
+    <t>uang parkir depan gedung HFS</t>
+  </si>
+  <si>
+    <t>uang parkir mobil</t>
+  </si>
+  <si>
+    <t>TOTAL</t>
+  </si>
+  <si>
+    <t>*dimulai tanggal 03 november 2021</t>
+  </si>
+  <si>
+    <t>*November 2021</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sisa saldo nota dari bulan oktober </t>
+  </si>
+  <si>
+    <t>uang masuk dari ce nanda (uang kas kecil asrama)</t>
+  </si>
+  <si>
+    <t>uang beli galon aqua (10 galon)</t>
+  </si>
+  <si>
+    <t>uang beli helm motor model kepala capung</t>
+  </si>
+  <si>
+    <t>uang beli bensin motor pertalite</t>
+  </si>
+  <si>
+    <t>hosea sama peter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">uang beli setrika maspion </t>
+  </si>
+  <si>
+    <t>uang grab cewek vaksin (berangkat - pulang)</t>
+  </si>
+  <si>
+    <t>fatma sama mega tobigo</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
+  <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
     <numFmt numFmtId="165" formatCode="_([$Rp-421]* #,##0.00_);_([$Rp-421]* \(#,##0.00\);_([$Rp-421]* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="166" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -224,6 +319,20 @@
       <family val="2"/>
       <scheme val="major"/>
     </font>
+    <font>
+      <sz val="20"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="24"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -252,7 +361,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -269,10 +378,27 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="17" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -592,8 +718,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1137C53-0063-4FE4-9637-7E05AFF16C56}">
   <dimension ref="A1:O76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="80" zoomScaleNormal="80" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="E38" sqref="E38"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -602,19 +728,19 @@
     <col min="3" max="3" width="31.42578125" customWidth="1"/>
     <col min="4" max="4" width="33.85546875" customWidth="1"/>
     <col min="5" max="5" width="27.85546875" customWidth="1"/>
-    <col min="6" max="6" width="44.5703125" customWidth="1"/>
+    <col min="6" max="6" width="70" customWidth="1"/>
     <col min="7" max="7" width="29.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
+      <c r="B1" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
       <c r="H1" s="2"/>
       <c r="I1" s="2"/>
       <c r="J1" s="2"/>
@@ -625,12 +751,12 @@
       <c r="O1" s="2"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B2" s="8"/>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
-      <c r="G2" s="8"/>
+      <c r="B2" s="10"/>
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="10"/>
+      <c r="G2" s="10"/>
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
       <c r="J2" s="2"/>
@@ -641,12 +767,12 @@
       <c r="O2" s="2"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B3" s="8"/>
-      <c r="C3" s="8"/>
-      <c r="D3" s="8"/>
-      <c r="E3" s="8"/>
-      <c r="F3" s="8"/>
-      <c r="G3" s="8"/>
+      <c r="B3" s="10"/>
+      <c r="C3" s="10"/>
+      <c r="D3" s="10"/>
+      <c r="E3" s="10"/>
+      <c r="F3" s="10"/>
+      <c r="G3" s="10"/>
       <c r="H3" s="2"/>
       <c r="I3" s="2"/>
       <c r="J3" s="2"/>
@@ -657,12 +783,12 @@
       <c r="O3" s="2"/>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B4" s="8"/>
-      <c r="C4" s="8"/>
-      <c r="D4" s="8"/>
-      <c r="E4" s="8"/>
-      <c r="F4" s="8"/>
-      <c r="G4" s="8"/>
+      <c r="B4" s="10"/>
+      <c r="C4" s="10"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="10"/>
+      <c r="G4" s="10"/>
       <c r="H4" s="2"/>
       <c r="I4" s="2"/>
       <c r="J4" s="2"/>
@@ -673,14 +799,14 @@
       <c r="O4" s="2"/>
     </row>
     <row r="5" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="9" t="s">
+      <c r="B5" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="9"/>
-      <c r="D5" s="9"/>
-      <c r="E5" s="9"/>
-      <c r="F5" s="9"/>
-      <c r="G5" s="9"/>
+      <c r="C5" s="11"/>
+      <c r="D5" s="11"/>
+      <c r="E5" s="11"/>
+      <c r="F5" s="11"/>
+      <c r="G5" s="11"/>
       <c r="H5" s="3"/>
       <c r="I5" s="3"/>
       <c r="J5" s="3"/>
@@ -691,12 +817,12 @@
       <c r="O5" s="3"/>
     </row>
     <row r="6" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="9"/>
-      <c r="C6" s="9"/>
-      <c r="D6" s="9"/>
-      <c r="E6" s="9"/>
-      <c r="F6" s="9"/>
-      <c r="G6" s="9"/>
+      <c r="B6" s="11"/>
+      <c r="C6" s="11"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="11"/>
+      <c r="F6" s="11"/>
+      <c r="G6" s="11"/>
       <c r="H6" s="3"/>
       <c r="I6" s="3"/>
       <c r="J6" s="3"/>
@@ -1012,7 +1138,7 @@
         <v>67400</v>
       </c>
       <c r="E20" s="6">
-        <f t="shared" ref="E20:E40" si="1">E19+C20-D20</f>
+        <f t="shared" ref="E20:E59" si="1">E19+C20-D20</f>
         <v>414200</v>
       </c>
       <c r="F20" t="s">
@@ -1479,97 +1605,526 @@
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B40" s="7"/>
-      <c r="C40" s="6"/>
+      <c r="A40">
+        <v>32</v>
+      </c>
+      <c r="B40" s="7">
+        <v>44491</v>
+      </c>
+      <c r="C40" s="6">
+        <v>100000</v>
+      </c>
+      <c r="D40" s="6">
+        <v>0</v>
+      </c>
       <c r="E40" s="6">
         <f t="shared" si="1"/>
-        <v>34600</v>
+        <v>134600</v>
+      </c>
+      <c r="F40" t="s">
+        <v>8</v>
+      </c>
+      <c r="G40" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B41" s="7"/>
-      <c r="C41" s="6"/>
-      <c r="E41" s="6"/>
+      <c r="A41">
+        <v>33</v>
+      </c>
+      <c r="B41" s="7">
+        <v>44491</v>
+      </c>
+      <c r="C41" s="6">
+        <v>0</v>
+      </c>
+      <c r="D41" s="6">
+        <v>78000</v>
+      </c>
+      <c r="E41" s="6">
+        <f t="shared" si="1"/>
+        <v>56600</v>
+      </c>
+      <c r="F41" t="s">
+        <v>41</v>
+      </c>
+      <c r="G41" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B42" s="7"/>
-      <c r="C42" s="6"/>
+      <c r="A42">
+        <v>34</v>
+      </c>
+      <c r="B42" s="7">
+        <v>44491</v>
+      </c>
+      <c r="C42" s="6">
+        <v>0</v>
+      </c>
+      <c r="D42" s="6">
+        <v>35900</v>
+      </c>
+      <c r="E42" s="6">
+        <f t="shared" si="1"/>
+        <v>20700</v>
+      </c>
+      <c r="F42" t="s">
+        <v>48</v>
+      </c>
+      <c r="G42" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B43" s="7"/>
-      <c r="C43" s="6"/>
+      <c r="A43">
+        <v>35</v>
+      </c>
+      <c r="B43" s="7">
+        <v>44491</v>
+      </c>
+      <c r="C43" s="6">
+        <v>0</v>
+      </c>
+      <c r="D43" s="6">
+        <v>2000</v>
+      </c>
+      <c r="E43" s="6">
+        <f t="shared" si="1"/>
+        <v>18700</v>
+      </c>
+      <c r="F43" t="s">
+        <v>38</v>
+      </c>
+      <c r="G43" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B44" s="7"/>
-      <c r="C44" s="6"/>
+      <c r="A44">
+        <v>36</v>
+      </c>
+      <c r="B44" s="7">
+        <v>44491</v>
+      </c>
+      <c r="C44" s="6">
+        <v>500000</v>
+      </c>
+      <c r="D44" s="6">
+        <v>0</v>
+      </c>
+      <c r="E44" s="6">
+        <f t="shared" si="1"/>
+        <v>518700</v>
+      </c>
+      <c r="F44" t="s">
+        <v>50</v>
+      </c>
+      <c r="G44" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B45" s="7"/>
-      <c r="C45" s="6"/>
+      <c r="A45">
+        <v>37</v>
+      </c>
+      <c r="B45" s="7">
+        <v>44492</v>
+      </c>
+      <c r="C45" s="6">
+        <v>0</v>
+      </c>
+      <c r="D45" s="6">
+        <v>20000</v>
+      </c>
+      <c r="E45" s="6">
+        <f t="shared" si="1"/>
+        <v>498700</v>
+      </c>
+      <c r="F45" t="s">
+        <v>51</v>
+      </c>
+      <c r="G45" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B46" s="7"/>
-      <c r="C46" s="6"/>
+      <c r="A46">
+        <v>38</v>
+      </c>
+      <c r="B46" s="7">
+        <v>44492</v>
+      </c>
+      <c r="C46" s="6">
+        <v>0</v>
+      </c>
+      <c r="D46" s="6">
+        <v>10000</v>
+      </c>
+      <c r="E46" s="6">
+        <f t="shared" si="1"/>
+        <v>488700</v>
+      </c>
+      <c r="F46" t="s">
+        <v>52</v>
+      </c>
+      <c r="G46" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B47" s="7"/>
-      <c r="C47" s="6"/>
+      <c r="A47">
+        <v>39</v>
+      </c>
+      <c r="B47" s="7">
+        <v>44492</v>
+      </c>
+      <c r="C47" s="6">
+        <v>0</v>
+      </c>
+      <c r="D47" s="6">
+        <v>81300</v>
+      </c>
+      <c r="E47" s="6">
+        <f t="shared" si="1"/>
+        <v>407400</v>
+      </c>
+      <c r="F47" t="s">
+        <v>53</v>
+      </c>
+      <c r="G47" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B48" s="7"/>
-      <c r="C48" s="6"/>
-    </row>
-    <row r="49" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B49" s="7"/>
-      <c r="C49" s="6"/>
-    </row>
-    <row r="50" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B50" s="7"/>
-      <c r="C50" s="6"/>
-    </row>
-    <row r="51" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B51" s="7"/>
-      <c r="C51" s="6"/>
-    </row>
-    <row r="52" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B52" s="7"/>
-      <c r="C52" s="6"/>
-    </row>
-    <row r="53" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B53" s="7"/>
-      <c r="C53" s="6"/>
-    </row>
-    <row r="54" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B54" s="7"/>
-    </row>
-    <row r="55" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B55" s="7"/>
-    </row>
-    <row r="56" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B56" s="7"/>
-    </row>
-    <row r="57" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B57" s="7"/>
-    </row>
-    <row r="58" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B58" s="7"/>
-    </row>
-    <row r="59" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B59" s="7"/>
-    </row>
-    <row r="60" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B60" s="7"/>
-    </row>
-    <row r="61" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B61" s="7"/>
-    </row>
-    <row r="62" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B62" s="7"/>
-    </row>
-    <row r="63" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>40</v>
+      </c>
+      <c r="B48" s="7">
+        <v>44493</v>
+      </c>
+      <c r="C48" s="6">
+        <v>0</v>
+      </c>
+      <c r="D48" s="6">
+        <v>15000</v>
+      </c>
+      <c r="E48" s="6">
+        <f t="shared" si="1"/>
+        <v>392400</v>
+      </c>
+      <c r="F48" t="s">
+        <v>54</v>
+      </c>
+      <c r="G48" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>41</v>
+      </c>
+      <c r="B49" s="7">
+        <v>44493</v>
+      </c>
+      <c r="C49" s="6">
+        <v>0</v>
+      </c>
+      <c r="D49" s="6">
+        <v>22000</v>
+      </c>
+      <c r="E49" s="6">
+        <f t="shared" si="1"/>
+        <v>370400</v>
+      </c>
+      <c r="F49" t="s">
+        <v>56</v>
+      </c>
+      <c r="G49" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>42</v>
+      </c>
+      <c r="B50" s="7">
+        <v>44494</v>
+      </c>
+      <c r="C50" s="6">
+        <v>0</v>
+      </c>
+      <c r="D50" s="6">
+        <v>48000</v>
+      </c>
+      <c r="E50" s="6">
+        <f>E49+C50-D50</f>
+        <v>322400</v>
+      </c>
+      <c r="F50" t="s">
+        <v>57</v>
+      </c>
+      <c r="G50" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>43</v>
+      </c>
+      <c r="B51" s="7">
+        <v>44496</v>
+      </c>
+      <c r="C51" s="6">
+        <v>0</v>
+      </c>
+      <c r="D51" s="6">
+        <v>200000</v>
+      </c>
+      <c r="E51" s="6">
+        <f t="shared" si="1"/>
+        <v>122400</v>
+      </c>
+      <c r="F51" t="s">
+        <v>58</v>
+      </c>
+      <c r="G51" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>44</v>
+      </c>
+      <c r="B52" s="7">
+        <v>44496</v>
+      </c>
+      <c r="C52" s="6">
+        <v>0</v>
+      </c>
+      <c r="D52" s="6">
+        <v>83000</v>
+      </c>
+      <c r="E52" s="6">
+        <f t="shared" si="1"/>
+        <v>39400</v>
+      </c>
+      <c r="F52" t="s">
+        <v>59</v>
+      </c>
+      <c r="G52" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>45</v>
+      </c>
+      <c r="B53" s="7">
+        <v>44496</v>
+      </c>
+      <c r="C53" s="6">
+        <v>0</v>
+      </c>
+      <c r="D53" s="6">
+        <v>10000</v>
+      </c>
+      <c r="E53" s="6">
+        <f t="shared" si="1"/>
+        <v>29400</v>
+      </c>
+      <c r="F53" t="s">
+        <v>60</v>
+      </c>
+      <c r="G53" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>46</v>
+      </c>
+      <c r="B54" s="7">
+        <v>44497</v>
+      </c>
+      <c r="C54" s="6">
+        <v>0</v>
+      </c>
+      <c r="D54" s="6">
+        <v>10000</v>
+      </c>
+      <c r="E54" s="6">
+        <f t="shared" si="1"/>
+        <v>19400</v>
+      </c>
+      <c r="F54" t="s">
+        <v>61</v>
+      </c>
+      <c r="G54" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <v>47</v>
+      </c>
+      <c r="B55" s="7">
+        <v>44497</v>
+      </c>
+      <c r="C55" s="6">
+        <v>0</v>
+      </c>
+      <c r="D55" s="6">
+        <v>3000</v>
+      </c>
+      <c r="E55" s="6">
+        <f t="shared" si="1"/>
+        <v>16400</v>
+      </c>
+      <c r="F55" t="s">
+        <v>62</v>
+      </c>
+      <c r="G55" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <v>48</v>
+      </c>
+      <c r="B56" s="7">
+        <v>44499</v>
+      </c>
+      <c r="C56" s="6">
+        <v>0</v>
+      </c>
+      <c r="D56" s="6">
+        <v>15000</v>
+      </c>
+      <c r="E56" s="6">
+        <f t="shared" si="1"/>
+        <v>1400</v>
+      </c>
+      <c r="F56" t="s">
+        <v>63</v>
+      </c>
+      <c r="G56" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <v>49</v>
+      </c>
+      <c r="B57" s="7">
+        <v>44500</v>
+      </c>
+      <c r="C57" s="6">
+        <v>0</v>
+      </c>
+      <c r="D57" s="6">
+        <v>5000</v>
+      </c>
+      <c r="E57" s="6">
+        <f t="shared" si="1"/>
+        <v>-3600</v>
+      </c>
+      <c r="F57" t="s">
+        <v>65</v>
+      </c>
+      <c r="G57" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <v>50</v>
+      </c>
+      <c r="B58" s="7">
+        <v>44500</v>
+      </c>
+      <c r="C58" s="6">
+        <v>0</v>
+      </c>
+      <c r="D58" s="6">
+        <v>10000</v>
+      </c>
+      <c r="E58" s="6">
+        <f t="shared" si="1"/>
+        <v>-13600</v>
+      </c>
+      <c r="F58" t="s">
+        <v>61</v>
+      </c>
+      <c r="G58" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A59">
+        <v>51</v>
+      </c>
+      <c r="B59" s="7">
+        <v>44500</v>
+      </c>
+      <c r="C59" s="6">
+        <v>0</v>
+      </c>
+      <c r="D59" s="6">
+        <v>5000</v>
+      </c>
+      <c r="E59" s="6">
+        <f t="shared" si="1"/>
+        <v>-18600</v>
+      </c>
+      <c r="F59" t="s">
+        <v>66</v>
+      </c>
+      <c r="G59" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A60" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="B60" s="13"/>
+      <c r="C60" s="14">
+        <f>SUM(C9:C59)</f>
+        <v>2100000</v>
+      </c>
+      <c r="D60" s="14">
+        <f>SUM(D9:D59)</f>
+        <v>2118600</v>
+      </c>
+      <c r="E60" s="14">
+        <v>-18600</v>
+      </c>
+      <c r="F60" s="13"/>
+      <c r="G60" s="13"/>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A61" s="13"/>
+      <c r="B61" s="13"/>
+      <c r="C61" s="15"/>
+      <c r="D61" s="15"/>
+      <c r="E61" s="14"/>
+      <c r="F61" s="13"/>
+      <c r="G61" s="13"/>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A62" s="13"/>
+      <c r="B62" s="13"/>
+      <c r="C62" s="15"/>
+      <c r="D62" s="15"/>
+      <c r="E62" s="14"/>
+      <c r="F62" s="13"/>
+      <c r="G62" s="13"/>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B63" s="7"/>
     </row>
-    <row r="64" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B64" s="7"/>
     </row>
     <row r="65" spans="2:2" x14ac:dyDescent="0.25">
@@ -1607,6 +2162,732 @@
     </row>
     <row r="76" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B76" s="7"/>
+    </row>
+  </sheetData>
+  <sheetProtection formatCells="0" formatColumns="0" formatRows="0"/>
+  <mergeCells count="7">
+    <mergeCell ref="B1:G4"/>
+    <mergeCell ref="B5:G6"/>
+    <mergeCell ref="A60:B62"/>
+    <mergeCell ref="C60:C62"/>
+    <mergeCell ref="D60:D62"/>
+    <mergeCell ref="E60:E62"/>
+    <mergeCell ref="F60:G62"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3BDAE0A9-9D0C-4DE2-9702-0E943FFDF5A6}">
+  <dimension ref="A1:G94"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="38.85546875" customWidth="1"/>
+    <col min="3" max="3" width="37.42578125" customWidth="1"/>
+    <col min="4" max="4" width="42.5703125" customWidth="1"/>
+    <col min="5" max="5" width="48.42578125" customWidth="1"/>
+    <col min="6" max="6" width="52" customWidth="1"/>
+    <col min="7" max="7" width="27.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B1" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B2" s="10"/>
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="10"/>
+      <c r="G2" s="10"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B3" s="10"/>
+      <c r="C3" s="10"/>
+      <c r="D3" s="10"/>
+      <c r="E3" s="10"/>
+      <c r="F3" s="10"/>
+      <c r="G3" s="10"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B4" s="10"/>
+      <c r="C4" s="10"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="10"/>
+      <c r="G4" s="10"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B5" s="16" t="s">
+        <v>69</v>
+      </c>
+      <c r="C5" s="11"/>
+      <c r="D5" s="11"/>
+      <c r="E5" s="11"/>
+      <c r="F5" s="11"/>
+      <c r="G5" s="11"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B6" s="11"/>
+      <c r="C6" s="11"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="11"/>
+      <c r="F6" s="11"/>
+      <c r="G6" s="11"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B7" s="5" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A8" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>1</v>
+      </c>
+      <c r="B9" s="8">
+        <v>44503</v>
+      </c>
+      <c r="C9" s="6">
+        <v>0</v>
+      </c>
+      <c r="D9" s="6">
+        <v>18600</v>
+      </c>
+      <c r="E9" s="6">
+        <f>C9-D9</f>
+        <v>-18600</v>
+      </c>
+      <c r="F9" t="s">
+        <v>70</v>
+      </c>
+      <c r="G9" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>2</v>
+      </c>
+      <c r="B10" s="8">
+        <v>44503</v>
+      </c>
+      <c r="C10" s="6">
+        <v>300000</v>
+      </c>
+      <c r="D10" s="6">
+        <v>0</v>
+      </c>
+      <c r="E10" s="6">
+        <f>E9+C10-D10</f>
+        <v>281400</v>
+      </c>
+      <c r="F10" t="s">
+        <v>71</v>
+      </c>
+      <c r="G10" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>3</v>
+      </c>
+      <c r="B11" s="8">
+        <v>44503</v>
+      </c>
+      <c r="C11" s="6">
+        <v>0</v>
+      </c>
+      <c r="D11" s="6">
+        <v>83000</v>
+      </c>
+      <c r="E11" s="6">
+        <f>E10+C11-D11</f>
+        <v>198400</v>
+      </c>
+      <c r="F11" t="s">
+        <v>72</v>
+      </c>
+      <c r="G11" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>4</v>
+      </c>
+      <c r="B12" s="8">
+        <v>44503</v>
+      </c>
+      <c r="C12" s="6">
+        <v>700000</v>
+      </c>
+      <c r="D12" s="6">
+        <v>0</v>
+      </c>
+      <c r="E12" s="6">
+        <f t="shared" ref="E12:E16" si="0">E11+C12-D12</f>
+        <v>898400</v>
+      </c>
+      <c r="F12" t="s">
+        <v>71</v>
+      </c>
+      <c r="G12" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>5</v>
+      </c>
+      <c r="B13" s="8">
+        <v>44503</v>
+      </c>
+      <c r="C13" s="6">
+        <v>0</v>
+      </c>
+      <c r="D13" s="6">
+        <v>150000</v>
+      </c>
+      <c r="E13" s="6">
+        <f t="shared" si="0"/>
+        <v>748400</v>
+      </c>
+      <c r="F13" t="s">
+        <v>73</v>
+      </c>
+      <c r="G13" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>6</v>
+      </c>
+      <c r="B14" s="8">
+        <v>44503</v>
+      </c>
+      <c r="C14" s="6">
+        <v>0</v>
+      </c>
+      <c r="D14" s="6">
+        <v>15000</v>
+      </c>
+      <c r="E14" s="6">
+        <f t="shared" si="0"/>
+        <v>733400</v>
+      </c>
+      <c r="F14" t="s">
+        <v>74</v>
+      </c>
+      <c r="G14" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>7</v>
+      </c>
+      <c r="B15" s="8">
+        <v>44503</v>
+      </c>
+      <c r="C15" s="6">
+        <v>0</v>
+      </c>
+      <c r="D15" s="6">
+        <v>150000</v>
+      </c>
+      <c r="E15" s="6">
+        <f t="shared" si="0"/>
+        <v>583400</v>
+      </c>
+      <c r="F15" t="s">
+        <v>76</v>
+      </c>
+      <c r="G15" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B16" s="8">
+        <v>44504</v>
+      </c>
+      <c r="C16" s="6">
+        <v>0</v>
+      </c>
+      <c r="D16" s="6">
+        <v>80000</v>
+      </c>
+      <c r="E16" s="6">
+        <f>E15+C16-D16</f>
+        <v>503400</v>
+      </c>
+      <c r="F16" t="s">
+        <v>77</v>
+      </c>
+      <c r="G16" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="17" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C17" s="6"/>
+      <c r="D17" s="6"/>
+      <c r="E17" s="6">
+        <f t="shared" ref="E17:E44" si="1">E16+C17-D17</f>
+        <v>503400</v>
+      </c>
+    </row>
+    <row r="18" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C18" s="6"/>
+      <c r="D18" s="6"/>
+      <c r="E18" s="6">
+        <f t="shared" si="1"/>
+        <v>503400</v>
+      </c>
+    </row>
+    <row r="19" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C19" s="6"/>
+      <c r="D19" s="6"/>
+      <c r="E19" s="6">
+        <f t="shared" si="1"/>
+        <v>503400</v>
+      </c>
+    </row>
+    <row r="20" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C20" s="6"/>
+      <c r="D20" s="6"/>
+      <c r="E20" s="6">
+        <f t="shared" si="1"/>
+        <v>503400</v>
+      </c>
+    </row>
+    <row r="21" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C21" s="6"/>
+      <c r="D21" s="6"/>
+      <c r="E21" s="6">
+        <f t="shared" si="1"/>
+        <v>503400</v>
+      </c>
+    </row>
+    <row r="22" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C22" s="6"/>
+      <c r="D22" s="6"/>
+      <c r="E22" s="6">
+        <f t="shared" si="1"/>
+        <v>503400</v>
+      </c>
+    </row>
+    <row r="23" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C23" s="6"/>
+      <c r="D23" s="6"/>
+      <c r="E23" s="6">
+        <f t="shared" si="1"/>
+        <v>503400</v>
+      </c>
+    </row>
+    <row r="24" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C24" s="6"/>
+      <c r="D24" s="6"/>
+      <c r="E24" s="6">
+        <f t="shared" si="1"/>
+        <v>503400</v>
+      </c>
+    </row>
+    <row r="25" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C25" s="6"/>
+      <c r="D25" s="6"/>
+      <c r="E25" s="6">
+        <f t="shared" si="1"/>
+        <v>503400</v>
+      </c>
+    </row>
+    <row r="26" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C26" s="6"/>
+      <c r="D26" s="6"/>
+      <c r="E26" s="6">
+        <f t="shared" si="1"/>
+        <v>503400</v>
+      </c>
+    </row>
+    <row r="27" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C27" s="6"/>
+      <c r="D27" s="6"/>
+      <c r="E27" s="6">
+        <f t="shared" si="1"/>
+        <v>503400</v>
+      </c>
+    </row>
+    <row r="28" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C28" s="6"/>
+      <c r="D28" s="6"/>
+      <c r="E28" s="6">
+        <f t="shared" si="1"/>
+        <v>503400</v>
+      </c>
+    </row>
+    <row r="29" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C29" s="6"/>
+      <c r="D29" s="6"/>
+      <c r="E29" s="6">
+        <f t="shared" si="1"/>
+        <v>503400</v>
+      </c>
+    </row>
+    <row r="30" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C30" s="6"/>
+      <c r="D30" s="6"/>
+      <c r="E30" s="6">
+        <f t="shared" si="1"/>
+        <v>503400</v>
+      </c>
+    </row>
+    <row r="31" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C31" s="6"/>
+      <c r="D31" s="6"/>
+      <c r="E31" s="6">
+        <f t="shared" si="1"/>
+        <v>503400</v>
+      </c>
+    </row>
+    <row r="32" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C32" s="6"/>
+      <c r="D32" s="6"/>
+      <c r="E32" s="6">
+        <f t="shared" si="1"/>
+        <v>503400</v>
+      </c>
+    </row>
+    <row r="33" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C33" s="6"/>
+      <c r="D33" s="6"/>
+      <c r="E33" s="6">
+        <f t="shared" si="1"/>
+        <v>503400</v>
+      </c>
+    </row>
+    <row r="34" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C34" s="6"/>
+      <c r="D34" s="6"/>
+      <c r="E34" s="6">
+        <f t="shared" si="1"/>
+        <v>503400</v>
+      </c>
+    </row>
+    <row r="35" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C35" s="6"/>
+      <c r="D35" s="6"/>
+      <c r="E35" s="6">
+        <f t="shared" si="1"/>
+        <v>503400</v>
+      </c>
+    </row>
+    <row r="36" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C36" s="6"/>
+      <c r="D36" s="6"/>
+      <c r="E36" s="6">
+        <f t="shared" si="1"/>
+        <v>503400</v>
+      </c>
+    </row>
+    <row r="37" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C37" s="6"/>
+      <c r="D37" s="6"/>
+      <c r="E37" s="6">
+        <f t="shared" si="1"/>
+        <v>503400</v>
+      </c>
+    </row>
+    <row r="38" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C38" s="6"/>
+      <c r="D38" s="6"/>
+      <c r="E38" s="6">
+        <f t="shared" si="1"/>
+        <v>503400</v>
+      </c>
+    </row>
+    <row r="39" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C39" s="6"/>
+      <c r="D39" s="6"/>
+      <c r="E39" s="6">
+        <f t="shared" si="1"/>
+        <v>503400</v>
+      </c>
+    </row>
+    <row r="40" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C40" s="6"/>
+      <c r="D40" s="6"/>
+      <c r="E40" s="6">
+        <f t="shared" si="1"/>
+        <v>503400</v>
+      </c>
+    </row>
+    <row r="41" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C41" s="6"/>
+      <c r="D41" s="6"/>
+      <c r="E41" s="6">
+        <f t="shared" si="1"/>
+        <v>503400</v>
+      </c>
+    </row>
+    <row r="42" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C42" s="9"/>
+      <c r="D42" s="6"/>
+      <c r="E42" s="6">
+        <f t="shared" si="1"/>
+        <v>503400</v>
+      </c>
+    </row>
+    <row r="43" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C43" s="9"/>
+      <c r="D43" s="6"/>
+      <c r="E43" s="6">
+        <f t="shared" si="1"/>
+        <v>503400</v>
+      </c>
+    </row>
+    <row r="44" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C44" s="9"/>
+      <c r="D44" s="6"/>
+      <c r="E44" s="6">
+        <f t="shared" si="1"/>
+        <v>503400</v>
+      </c>
+    </row>
+    <row r="45" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="D45" s="6"/>
+      <c r="E45" s="6"/>
+    </row>
+    <row r="46" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="D46" s="6"/>
+      <c r="E46" s="6"/>
+    </row>
+    <row r="47" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="D47" s="6"/>
+      <c r="E47" s="6"/>
+    </row>
+    <row r="48" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="D48" s="6"/>
+      <c r="E48" s="6"/>
+    </row>
+    <row r="49" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D49" s="6"/>
+      <c r="E49" s="6"/>
+    </row>
+    <row r="50" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D50" s="6"/>
+      <c r="E50" s="6"/>
+    </row>
+    <row r="51" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D51" s="6"/>
+      <c r="E51" s="6"/>
+    </row>
+    <row r="52" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D52" s="6"/>
+      <c r="E52" s="6"/>
+    </row>
+    <row r="53" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D53" s="6"/>
+      <c r="E53" s="6"/>
+    </row>
+    <row r="54" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D54" s="6"/>
+      <c r="E54" s="6"/>
+    </row>
+    <row r="55" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D55" s="6"/>
+      <c r="E55" s="6"/>
+    </row>
+    <row r="56" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D56" s="6"/>
+      <c r="E56" s="6"/>
+    </row>
+    <row r="57" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D57" s="6"/>
+      <c r="E57" s="6"/>
+    </row>
+    <row r="58" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D58" s="6"/>
+      <c r="E58" s="6"/>
+    </row>
+    <row r="59" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D59" s="6"/>
+      <c r="E59" s="6"/>
+    </row>
+    <row r="60" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D60" s="6"/>
+      <c r="E60" s="6"/>
+    </row>
+    <row r="61" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D61" s="6"/>
+      <c r="E61" s="6"/>
+    </row>
+    <row r="62" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D62" s="6"/>
+      <c r="E62" s="6"/>
+    </row>
+    <row r="63" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D63" s="6"/>
+      <c r="E63" s="6"/>
+    </row>
+    <row r="64" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D64" s="6"/>
+      <c r="E64" s="6"/>
+    </row>
+    <row r="65" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D65" s="6"/>
+      <c r="E65" s="6"/>
+    </row>
+    <row r="66" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D66" s="6"/>
+      <c r="E66" s="6"/>
+    </row>
+    <row r="67" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D67" s="6"/>
+      <c r="E67" s="6"/>
+    </row>
+    <row r="68" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D68" s="6"/>
+      <c r="E68" s="6"/>
+    </row>
+    <row r="69" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D69" s="6"/>
+      <c r="E69" s="6"/>
+    </row>
+    <row r="70" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D70" s="6"/>
+      <c r="E70" s="6"/>
+    </row>
+    <row r="71" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D71" s="6"/>
+      <c r="E71" s="6"/>
+    </row>
+    <row r="72" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D72" s="6"/>
+      <c r="E72" s="6"/>
+    </row>
+    <row r="73" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D73" s="6"/>
+      <c r="E73" s="6"/>
+    </row>
+    <row r="74" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D74" s="6"/>
+      <c r="E74" s="6"/>
+    </row>
+    <row r="75" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D75" s="6"/>
+      <c r="E75" s="6"/>
+    </row>
+    <row r="76" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D76" s="6"/>
+      <c r="E76" s="6"/>
+    </row>
+    <row r="77" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D77" s="6"/>
+      <c r="E77" s="6"/>
+    </row>
+    <row r="78" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D78" s="6"/>
+      <c r="E78" s="6"/>
+    </row>
+    <row r="79" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D79" s="6"/>
+      <c r="E79" s="6"/>
+    </row>
+    <row r="80" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D80" s="6"/>
+      <c r="E80" s="6"/>
+    </row>
+    <row r="81" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D81" s="6"/>
+      <c r="E81" s="6"/>
+    </row>
+    <row r="82" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D82" s="6"/>
+      <c r="E82" s="6"/>
+    </row>
+    <row r="83" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D83" s="6"/>
+      <c r="E83" s="6"/>
+    </row>
+    <row r="84" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D84" s="6"/>
+      <c r="E84" s="6"/>
+    </row>
+    <row r="85" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D85" s="6"/>
+      <c r="E85" s="6"/>
+    </row>
+    <row r="86" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D86" s="6"/>
+      <c r="E86" s="6"/>
+    </row>
+    <row r="87" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D87" s="6"/>
+      <c r="E87" s="6"/>
+    </row>
+    <row r="88" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D88" s="6"/>
+      <c r="E88" s="6"/>
+    </row>
+    <row r="89" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D89" s="6"/>
+      <c r="E89" s="6"/>
+    </row>
+    <row r="90" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D90" s="6"/>
+      <c r="E90" s="6"/>
+    </row>
+    <row r="91" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D91" s="6"/>
+      <c r="E91" s="6"/>
+    </row>
+    <row r="92" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D92" s="6"/>
+      <c r="E92" s="6"/>
+    </row>
+    <row r="93" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D93" s="6"/>
+      <c r="E93" s="6"/>
+    </row>
+    <row r="94" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="E94" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
13 11 2021 - part 2
</commit_message>
<xml_diff>
--- a/rekap data uang kas kecil - asrama.xlsx
+++ b/rekap data uang kas kecil - asrama.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yofandi Riki Winata\Documents\yofandi\rekap data - uang galon, parkir, bumbu asrama\uangasrama\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BB8DA56-ADD1-4588-B96A-677483E8B426}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7E99E51-9035-4A66-B62B-7E1A21A76E66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" activeTab="1" xr2:uid="{C456B771-9DF8-4725-AC5F-E2624C050843}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="100">
   <si>
     <t>Kas Kecil - Asrama STTHF</t>
   </si>
@@ -327,6 +327,15 @@
   </si>
   <si>
     <t>uang beli isi strapes</t>
+  </si>
+  <si>
+    <t>lunas</t>
+  </si>
+  <si>
+    <t>uang beli barang keperluan asrama di indogrosir</t>
+  </si>
+  <si>
+    <t>yofandi sama valen sama jhonan</t>
   </si>
 </sst>
 </file>
@@ -2239,10 +2248,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3BDAE0A9-9D0C-4DE2-9702-0E943FFDF5A6}">
-  <dimension ref="A1:J94"/>
+  <dimension ref="A1:K94"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B7" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView tabSelected="1" topLeftCell="B5" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2252,7 +2261,7 @@
     <col min="4" max="4" width="42.5703125" customWidth="1"/>
     <col min="5" max="5" width="48.42578125" customWidth="1"/>
     <col min="6" max="6" width="52" customWidth="1"/>
-    <col min="7" max="7" width="27.85546875" customWidth="1"/>
+    <col min="7" max="7" width="31.5703125" customWidth="1"/>
     <col min="8" max="8" width="13.85546875" customWidth="1"/>
     <col min="9" max="9" width="27.28515625" customWidth="1"/>
     <col min="10" max="10" width="20" customWidth="1"/>
@@ -2538,7 +2547,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -2563,7 +2572,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -2588,7 +2597,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -2613,7 +2622,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -2642,10 +2651,10 @@
       </c>
       <c r="J20" s="6">
         <f>SUM(C9:C44)</f>
-        <v>1850000</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+        <v>3100000</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -2670,7 +2679,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -2695,7 +2704,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -2729,8 +2738,11 @@
         <f>D23+D24+D25+D27+D28+D29+D30+D31+D32+D33</f>
         <v>340900</v>
       </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K23" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -2757,12 +2769,9 @@
       <c r="H24" t="s">
         <v>85</v>
       </c>
-      <c r="J24" s="6">
-        <f>SUM(D23:D33)</f>
-        <v>391200</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J24" s="6"/>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -2790,7 +2799,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -2818,7 +2827,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -2846,7 +2855,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -2874,7 +2883,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29">
         <f t="shared" si="0"/>
         <v>21</v>
@@ -2902,7 +2911,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30">
         <f t="shared" si="0"/>
         <v>22</v>
@@ -2930,7 +2939,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B31" s="8">
         <v>44509</v>
       </c>
@@ -2954,7 +2963,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B32" s="8">
         <v>44510</v>
       </c>
@@ -3087,27 +3096,66 @@
       </c>
     </row>
     <row r="38" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="C38" s="6"/>
-      <c r="D38" s="6"/>
+      <c r="B38" s="8">
+        <v>44513</v>
+      </c>
+      <c r="C38" s="6">
+        <v>1250000</v>
+      </c>
+      <c r="D38" s="6">
+        <v>0</v>
+      </c>
       <c r="E38" s="6">
         <f t="shared" si="2"/>
-        <v>274200</v>
+        <v>1524200</v>
+      </c>
+      <c r="F38" t="s">
+        <v>93</v>
+      </c>
+      <c r="G38" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="39" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="C39" s="6"/>
-      <c r="D39" s="6"/>
+      <c r="B39" s="8">
+        <v>44513</v>
+      </c>
+      <c r="C39" s="6">
+        <v>0</v>
+      </c>
+      <c r="D39" s="6">
+        <v>1576500</v>
+      </c>
       <c r="E39" s="6">
         <f t="shared" si="2"/>
-        <v>274200</v>
+        <v>-52300</v>
+      </c>
+      <c r="F39" t="s">
+        <v>98</v>
+      </c>
+      <c r="G39" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="40" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="C40" s="6"/>
-      <c r="D40" s="6"/>
+      <c r="B40" s="8">
+        <v>44513</v>
+      </c>
+      <c r="C40" s="6">
+        <v>0</v>
+      </c>
+      <c r="D40" s="6">
+        <v>15000</v>
+      </c>
       <c r="E40" s="6">
         <f t="shared" si="2"/>
-        <v>274200</v>
+        <v>-67300</v>
+      </c>
+      <c r="F40" t="s">
+        <v>74</v>
+      </c>
+      <c r="G40" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="41" spans="2:8" x14ac:dyDescent="0.25">
@@ -3115,7 +3163,7 @@
       <c r="D41" s="6"/>
       <c r="E41" s="6">
         <f t="shared" si="2"/>
-        <v>274200</v>
+        <v>-67300</v>
       </c>
     </row>
     <row r="42" spans="2:8" x14ac:dyDescent="0.25">
@@ -3123,7 +3171,7 @@
       <c r="D42" s="6"/>
       <c r="E42" s="6">
         <f t="shared" si="2"/>
-        <v>274200</v>
+        <v>-67300</v>
       </c>
     </row>
     <row r="43" spans="2:8" x14ac:dyDescent="0.25">
@@ -3131,7 +3179,7 @@
       <c r="D43" s="6"/>
       <c r="E43" s="6">
         <f t="shared" si="2"/>
-        <v>274200</v>
+        <v>-67300</v>
       </c>
     </row>
     <row r="44" spans="2:8" x14ac:dyDescent="0.25">
@@ -3139,7 +3187,7 @@
       <c r="D44" s="6"/>
       <c r="E44" s="6">
         <f t="shared" si="2"/>
-        <v>274200</v>
+        <v>-67300</v>
       </c>
     </row>
     <row r="45" spans="2:8" x14ac:dyDescent="0.25">

</xml_diff>